<commit_message>
20241110 funciones de toma de datos de cimentacion
</commit_message>
<xml_diff>
--- a/datos_cimentacion.xlsx
+++ b/datos_cimentacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\germa\Documentos\Programacion\Python\CargaAdmisible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365EF2A9-C678-421C-97AD-91F737836344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF53672-80D1-4955-B93B-1610BB9CEA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>B[m]</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Forma</t>
+  </si>
+  <si>
+    <t>FS</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +389,7 @@
     <col min="6" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,8 +414,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1.5</v>
       </c>
@@ -436,6 +442,9 @@
       </c>
       <c r="H2" s="1">
         <v>10</v>
+      </c>
+      <c r="I2" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>